<commit_message>
Correções no arquivo aniversariantes.php
</commit_message>
<xml_diff>
--- a/desafio-aniversariantes/202402.xlsx
+++ b/desafio-aniversariantes/202402.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\teste-estagio-php\desafio-aniversariantes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DE9D5B-FEC6-4FF3-9475-7C0966F2AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC59D75-DFA7-44C5-9522-61B8351995CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,10 +91,10 @@
     <t>Tomás Araujo Dias</t>
   </si>
   <si>
-    <t>Teste</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rodrigo </t>
+  </si>
+  <si>
+    <t>Leo</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -629,26 +629,26 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>38471</v>
       </c>
       <c r="C21" s="3">
-        <v>43943</v>
+        <v>43950</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="4">
         <v>37951</v>
       </c>
-      <c r="C22" s="4">
-        <v>45045</v>
+      <c r="C22" s="3">
+        <v>43950</v>
       </c>
       <c r="E22" s="5"/>
     </row>

</xml_diff>